<commit_message>
adding in all TPC3 @ 25C data
</commit_message>
<xml_diff>
--- a/data-raw/tpc-july29/fist_01.xlsx
+++ b/data-raw/tpc-july29/fist_01.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Imaging Controller\Desktop\Ijeoma\TPC3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2B051358-6520-4DDB-883F-861D71F20940}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{52F0DC2A-4421-41DF-9B4C-49AA35AF7627}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16005" windowHeight="10125" xr2:uid="{FF9ECED7-4841-4BED-938D-299DB5C94CAF}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16005" windowHeight="10125" xr2:uid="{55415A64-96C0-4F62-9E96-007F80B75154}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -103,79 +103,79 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FF6FA9D6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF8DBCE0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFC9E0F4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FF5197CC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF60A0D1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7EB2DB"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF3385C2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFBAD7EF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF247CBD"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFABCEEA"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD8E9F9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFE8F3FF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFABCEEA"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFD8E9F9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF8DBCE0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFBAD7EF"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF7EB2DB"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FF428EC7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF60A0D1"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF247CBD"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF5197CC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF6FA9D6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF3385C2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -230,14 +230,14 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -573,7 +573,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FC3DD01-A720-4B93-8362-FE840ADFA48A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F642C536-FE04-42BB-A022-8A9412387B9E}">
   <dimension ref="A1:N9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -624,42 +624,42 @@
         <v>0</v>
       </c>
       <c r="B2" s="3">
-        <v>25</v>
-      </c>
-      <c r="C2" s="4">
+        <v>17</v>
+      </c>
+      <c r="C2" s="3">
+        <v>18</v>
+      </c>
+      <c r="D2" s="3">
+        <v>17</v>
+      </c>
+      <c r="E2" s="3">
+        <v>17</v>
+      </c>
+      <c r="F2" s="4">
+        <v>22</v>
+      </c>
+      <c r="G2" s="3">
+        <v>17</v>
+      </c>
+      <c r="H2" s="5">
         <v>19</v>
       </c>
-      <c r="D2" s="5">
-        <v>14</v>
-      </c>
-      <c r="E2" s="4">
-        <v>19</v>
-      </c>
-      <c r="F2" s="6">
+      <c r="I2" s="6">
+        <v>13</v>
+      </c>
+      <c r="J2" s="7">
+        <v>26</v>
+      </c>
+      <c r="K2" s="4">
         <v>22</v>
       </c>
-      <c r="G2" s="7">
-        <v>16</v>
-      </c>
-      <c r="H2" s="3">
-        <v>25</v>
-      </c>
-      <c r="I2" s="7">
-        <v>16</v>
-      </c>
-      <c r="J2" s="8">
-        <v>27</v>
-      </c>
-      <c r="K2" s="9">
-        <v>21</v>
-      </c>
-      <c r="L2" s="9">
-        <v>21</v>
-      </c>
-      <c r="M2" s="6">
-        <v>22</v>
-      </c>
-      <c r="N2" s="10">
+      <c r="L2" s="4">
+        <v>23</v>
+      </c>
+      <c r="M2" s="4">
+        <v>23</v>
+      </c>
+      <c r="N2" s="8">
         <v>440670</v>
       </c>
     </row>
@@ -667,43 +667,43 @@
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="6">
+      <c r="B3" s="4">
+        <v>23</v>
+      </c>
+      <c r="C3" s="4">
         <v>22</v>
       </c>
-      <c r="C3" s="11">
-        <v>28</v>
-      </c>
-      <c r="D3" s="3">
+      <c r="D3" s="6">
+        <v>13</v>
+      </c>
+      <c r="E3" s="9">
         <v>24</v>
       </c>
-      <c r="E3" s="12">
-        <v>36</v>
-      </c>
-      <c r="F3" s="9">
+      <c r="F3" s="10">
+        <v>21</v>
+      </c>
+      <c r="G3" s="11">
+        <v>29</v>
+      </c>
+      <c r="H3" s="5">
         <v>20</v>
       </c>
-      <c r="G3" s="13">
-        <v>31</v>
-      </c>
-      <c r="H3" s="6">
+      <c r="I3" s="5">
+        <v>19</v>
+      </c>
+      <c r="J3" s="10">
+        <v>21</v>
+      </c>
+      <c r="K3" s="3">
+        <v>18</v>
+      </c>
+      <c r="L3" s="4">
         <v>22</v>
       </c>
-      <c r="I3" s="13">
-        <v>32</v>
-      </c>
-      <c r="J3" s="8">
-        <v>27</v>
-      </c>
-      <c r="K3" s="12">
-        <v>35</v>
-      </c>
-      <c r="L3" s="6">
-        <v>23</v>
-      </c>
-      <c r="M3" s="3">
-        <v>24</v>
-      </c>
-      <c r="N3" s="10">
+      <c r="M3" s="5">
+        <v>20</v>
+      </c>
+      <c r="N3" s="8">
         <v>440670</v>
       </c>
     </row>
@@ -711,43 +711,43 @@
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="12">
+        <v>14</v>
+      </c>
+      <c r="C4" s="3">
+        <v>17</v>
+      </c>
+      <c r="D4" s="13">
+        <v>31</v>
+      </c>
+      <c r="E4" s="12">
+        <v>15</v>
+      </c>
+      <c r="F4" s="5">
+        <v>20</v>
+      </c>
+      <c r="G4" s="12">
+        <v>15</v>
+      </c>
+      <c r="H4" s="9">
         <v>24</v>
       </c>
-      <c r="C4" s="6">
-        <v>22</v>
-      </c>
-      <c r="D4" s="14">
-        <v>40</v>
-      </c>
-      <c r="E4" s="8">
-        <v>27</v>
-      </c>
-      <c r="F4" s="13">
-        <v>31</v>
-      </c>
-      <c r="G4" s="3">
-        <v>24</v>
-      </c>
-      <c r="H4" s="13">
-        <v>31</v>
-      </c>
-      <c r="I4" s="8">
-        <v>26</v>
-      </c>
-      <c r="J4" s="12">
-        <v>36</v>
-      </c>
-      <c r="K4" s="4">
-        <v>19</v>
-      </c>
-      <c r="L4" s="15">
-        <v>33</v>
-      </c>
-      <c r="M4" s="16">
-        <v>30</v>
-      </c>
-      <c r="N4" s="10">
+      <c r="I4" s="14">
+        <v>16</v>
+      </c>
+      <c r="J4" s="11">
+        <v>28</v>
+      </c>
+      <c r="K4" s="12">
+        <v>15</v>
+      </c>
+      <c r="L4" s="5">
+        <v>20</v>
+      </c>
+      <c r="M4" s="10">
+        <v>21</v>
+      </c>
+      <c r="N4" s="8">
         <v>440670</v>
       </c>
     </row>
@@ -755,43 +755,43 @@
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="4">
+      <c r="B5" s="10">
+        <v>21</v>
+      </c>
+      <c r="C5" s="10">
+        <v>21</v>
+      </c>
+      <c r="D5" s="10">
+        <v>21</v>
+      </c>
+      <c r="E5" s="3">
+        <v>18</v>
+      </c>
+      <c r="F5" s="5">
         <v>19</v>
       </c>
-      <c r="C5" s="9">
+      <c r="G5" s="7">
+        <v>25</v>
+      </c>
+      <c r="H5" s="5">
         <v>20</v>
       </c>
-      <c r="D5" s="8">
-        <v>26</v>
-      </c>
-      <c r="E5" s="13">
-        <v>32</v>
-      </c>
-      <c r="F5" s="9">
-        <v>20</v>
-      </c>
-      <c r="G5" s="11">
-        <v>28</v>
-      </c>
-      <c r="H5" s="4">
+      <c r="I5" s="3">
+        <v>18</v>
+      </c>
+      <c r="J5" s="10">
+        <v>21</v>
+      </c>
+      <c r="K5" s="5">
         <v>19</v>
       </c>
-      <c r="I5" s="16">
-        <v>30</v>
-      </c>
-      <c r="J5" s="8">
-        <v>26</v>
-      </c>
-      <c r="K5" s="17">
-        <v>38</v>
-      </c>
-      <c r="L5" s="16">
-        <v>29</v>
-      </c>
-      <c r="M5" s="9">
-        <v>21</v>
-      </c>
-      <c r="N5" s="10">
+      <c r="L5" s="5">
+        <v>19</v>
+      </c>
+      <c r="M5" s="4">
+        <v>22</v>
+      </c>
+      <c r="N5" s="8">
         <v>440670</v>
       </c>
     </row>
@@ -799,43 +799,43 @@
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="7">
+      <c r="B6" s="10">
+        <v>21</v>
+      </c>
+      <c r="C6" s="5">
+        <v>20</v>
+      </c>
+      <c r="D6" s="3">
+        <v>18</v>
+      </c>
+      <c r="E6" s="15">
+        <v>11</v>
+      </c>
+      <c r="F6" s="12">
+        <v>14</v>
+      </c>
+      <c r="G6" s="14">
         <v>16</v>
       </c>
-      <c r="C6" s="9">
-        <v>20</v>
-      </c>
-      <c r="D6" s="13">
-        <v>32</v>
-      </c>
-      <c r="E6" s="9">
-        <v>20</v>
-      </c>
-      <c r="F6" s="15">
-        <v>34</v>
-      </c>
-      <c r="G6" s="9">
-        <v>20</v>
-      </c>
-      <c r="H6" s="8">
+      <c r="H6" s="10">
+        <v>21</v>
+      </c>
+      <c r="I6" s="16">
+        <v>9</v>
+      </c>
+      <c r="J6" s="17">
         <v>27</v>
       </c>
-      <c r="I6" s="3">
-        <v>25</v>
-      </c>
-      <c r="J6" s="15">
-        <v>33</v>
-      </c>
-      <c r="K6" s="3">
+      <c r="K6" s="9">
         <v>24</v>
       </c>
-      <c r="L6" s="16">
-        <v>29</v>
-      </c>
-      <c r="M6" s="6">
-        <v>23</v>
-      </c>
-      <c r="N6" s="10">
+      <c r="L6" s="9">
+        <v>24</v>
+      </c>
+      <c r="M6" s="3">
+        <v>17</v>
+      </c>
+      <c r="N6" s="8">
         <v>440670</v>
       </c>
     </row>
@@ -843,43 +843,43 @@
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7" s="5">
+        <v>20</v>
+      </c>
+      <c r="C7" s="4">
+        <v>22</v>
+      </c>
+      <c r="D7" s="3">
+        <v>18</v>
+      </c>
+      <c r="E7" s="13">
+        <v>30</v>
+      </c>
+      <c r="F7" s="3">
+        <v>18</v>
+      </c>
+      <c r="G7" s="3">
+        <v>18</v>
+      </c>
+      <c r="H7" s="3">
+        <v>17</v>
+      </c>
+      <c r="I7" s="10">
+        <v>21</v>
+      </c>
+      <c r="J7" s="12">
+        <v>14</v>
+      </c>
+      <c r="K7" s="7">
         <v>25</v>
       </c>
-      <c r="C7" s="11">
-        <v>28</v>
-      </c>
-      <c r="D7" s="6">
-        <v>23</v>
-      </c>
-      <c r="E7" s="3">
-        <v>24</v>
-      </c>
-      <c r="F7" s="6">
-        <v>23</v>
-      </c>
-      <c r="G7" s="12">
-        <v>36</v>
-      </c>
-      <c r="H7" s="5">
-        <v>14</v>
-      </c>
-      <c r="I7" s="3">
-        <v>24</v>
-      </c>
-      <c r="J7" s="9">
-        <v>21</v>
-      </c>
-      <c r="K7" s="12">
-        <v>36</v>
-      </c>
-      <c r="L7" s="8">
-        <v>26</v>
-      </c>
-      <c r="M7" s="9">
-        <v>20</v>
-      </c>
-      <c r="N7" s="10">
+      <c r="L7" s="13">
+        <v>31</v>
+      </c>
+      <c r="M7" s="14">
+        <v>16</v>
+      </c>
+      <c r="N7" s="8">
         <v>440670</v>
       </c>
     </row>
@@ -888,42 +888,42 @@
         <v>6</v>
       </c>
       <c r="B8" s="3">
-        <v>24</v>
-      </c>
-      <c r="C8" s="6">
-        <v>22</v>
-      </c>
-      <c r="D8" s="8">
+        <v>18</v>
+      </c>
+      <c r="C8" s="12">
+        <v>14</v>
+      </c>
+      <c r="D8" s="11">
+        <v>28</v>
+      </c>
+      <c r="E8" s="3">
+        <v>17</v>
+      </c>
+      <c r="F8" s="3">
+        <v>18</v>
+      </c>
+      <c r="G8" s="10">
+        <v>21</v>
+      </c>
+      <c r="H8" s="7">
         <v>26</v>
       </c>
-      <c r="E8" s="3">
-        <v>24</v>
-      </c>
-      <c r="F8" s="15">
-        <v>33</v>
-      </c>
-      <c r="G8" s="8">
-        <v>26</v>
-      </c>
-      <c r="H8" s="15">
-        <v>34</v>
-      </c>
-      <c r="I8" s="4">
+      <c r="I8" s="5">
         <v>19</v>
       </c>
-      <c r="J8" s="12">
-        <v>35</v>
-      </c>
-      <c r="K8" s="9">
+      <c r="J8" s="3">
+        <v>17</v>
+      </c>
+      <c r="K8" s="14">
+        <v>16</v>
+      </c>
+      <c r="L8" s="13">
+        <v>30</v>
+      </c>
+      <c r="M8" s="5">
         <v>20</v>
       </c>
-      <c r="L8" s="12">
-        <v>36</v>
-      </c>
-      <c r="M8" s="9">
-        <v>20</v>
-      </c>
-      <c r="N8" s="10">
+      <c r="N8" s="8">
         <v>440670</v>
       </c>
     </row>
@@ -931,43 +931,43 @@
       <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="9">
-        <v>21</v>
-      </c>
-      <c r="C9" s="4">
+      <c r="B9" s="7">
+        <v>25</v>
+      </c>
+      <c r="C9" s="12">
+        <v>14</v>
+      </c>
+      <c r="D9" s="12">
+        <v>14</v>
+      </c>
+      <c r="E9" s="3">
+        <v>18</v>
+      </c>
+      <c r="F9" s="12">
+        <v>14</v>
+      </c>
+      <c r="G9" s="4">
+        <v>22</v>
+      </c>
+      <c r="H9" s="14">
+        <v>16</v>
+      </c>
+      <c r="I9" s="10">
+        <v>21</v>
+      </c>
+      <c r="J9" s="3">
+        <v>18</v>
+      </c>
+      <c r="K9" s="4">
+        <v>22</v>
+      </c>
+      <c r="L9" s="14">
+        <v>16</v>
+      </c>
+      <c r="M9" s="5">
         <v>19</v>
       </c>
-      <c r="D9" s="9">
-        <v>21</v>
-      </c>
-      <c r="E9" s="6">
-        <v>22</v>
-      </c>
-      <c r="F9" s="7">
-        <v>17</v>
-      </c>
-      <c r="G9" s="9">
-        <v>21</v>
-      </c>
-      <c r="H9" s="9">
-        <v>20</v>
-      </c>
-      <c r="I9" s="9">
-        <v>20</v>
-      </c>
-      <c r="J9" s="9">
-        <v>20</v>
-      </c>
-      <c r="K9" s="6">
-        <v>22</v>
-      </c>
-      <c r="L9" s="3">
-        <v>25</v>
-      </c>
-      <c r="M9" s="9">
-        <v>20</v>
-      </c>
-      <c r="N9" s="10">
+      <c r="N9" s="8">
         <v>440670</v>
       </c>
     </row>

</xml_diff>